<commit_message>
Code changes for Excel utility
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/qa7/testData.xlsx
+++ b/src/test/resources/test-data/qa7/testData.xlsx
@@ -5,24 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vigneshwaran.sesurag\Gradle\chatr-e2e-automation-2\src\test\resources\test-data\qa7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vigneshwaran.sesurag\Gradle\CPP_Automation-Chatr\src\test\resources\test-data\qa7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8D5DDE-1620-401C-B1D5-444520C1C7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8920E6-01EE-45B9-BE7E-EBEB810445A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Voucher" sheetId="2" r:id="rId1"/>
     <sheet name="NAC_DataCreation" sheetId="3" r:id="rId2"/>
-    <sheet name="EAS" sheetId="4" r:id="rId3"/>
-    <sheet name="CTNDATA" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="8" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId7"/>
-    <sheet name="NAC OLD" sheetId="9" r:id="rId8"/>
-    <sheet name="Voucher OLD" sheetId="10" r:id="rId9"/>
-    <sheet name="EAS OLD" sheetId="11" r:id="rId10"/>
+    <sheet name="NAC_Data" sheetId="12" r:id="rId3"/>
+    <sheet name="EAS" sheetId="4" r:id="rId4"/>
+    <sheet name="CTNDATA" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId8"/>
+    <sheet name="NAC OLD" sheetId="9" r:id="rId9"/>
+    <sheet name="Voucher OLD" sheetId="10" r:id="rId10"/>
+    <sheet name="EAS OLD" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="545">
   <si>
     <t>Voucher25</t>
   </si>
@@ -1677,6 +1678,9 @@
   </si>
   <si>
     <t>eas6</t>
+  </si>
+  <si>
+    <t>4169041183</t>
   </si>
 </sst>
 </file>
@@ -2803,6 +2807,1044 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6B3CDC-0AFC-4B53-A9D5-8ABE836A7404}">
+  <dimension ref="A1:N91"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.7109375" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="F2" t="s">
+        <v>341</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="H2" t="s">
+        <v>341</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="J2" t="s">
+        <v>341</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="L2" t="s">
+        <v>341</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="N2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3"/>
+      <c r="C3" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D3" t="s">
+        <v>341</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="F3" t="s">
+        <v>341</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="H3" t="s">
+        <v>341</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" t="s">
+        <v>341</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="L3" t="s">
+        <v>341</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="N3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4"/>
+      <c r="C4" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="D4" t="s">
+        <v>341</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="F4" t="s">
+        <v>341</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="H4" t="s">
+        <v>341</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" t="s">
+        <v>341</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="L4" t="s">
+        <v>341</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="N4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5"/>
+      <c r="C5" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="D5" t="s">
+        <v>341</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="F5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="H5" t="s">
+        <v>341</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5"/>
+      <c r="K5" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="L5" t="s">
+        <v>341</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="N5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6"/>
+      <c r="C6" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D6" t="s">
+        <v>341</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H6" t="s">
+        <v>341</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6"/>
+      <c r="K6" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="L6" t="s">
+        <v>341</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="N6" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7"/>
+      <c r="C7" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="D7" t="s">
+        <v>341</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="H7" t="s">
+        <v>341</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7"/>
+      <c r="K7" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="L7" t="s">
+        <v>341</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="N7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8"/>
+      <c r="C8" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="D8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="H8" t="s">
+        <v>341</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8"/>
+      <c r="K8" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="L8" t="s">
+        <v>341</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="N8" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9"/>
+      <c r="C9" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="D9" t="s">
+        <v>341</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9" s="7"/>
+      <c r="K9" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="L9" t="s">
+        <v>341</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="N9" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10"/>
+      <c r="C10" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="D10" t="s">
+        <v>341</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10" s="7"/>
+      <c r="K10" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="L10" t="s">
+        <v>341</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="N10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11"/>
+      <c r="C11" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="D11" t="s">
+        <v>341</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="H11"/>
+      <c r="K11" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="N11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12"/>
+      <c r="C12" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="D12" t="s">
+        <v>341</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="F12"/>
+      <c r="G12" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H12"/>
+      <c r="K12" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="N12" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13"/>
+      <c r="C13" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="D13"/>
+      <c r="E13" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="F13"/>
+      <c r="G13" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="H13"/>
+      <c r="K13" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="N13" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14"/>
+      <c r="C14" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="H14"/>
+      <c r="K14" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="N14" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15"/>
+      <c r="C15" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="D15"/>
+      <c r="E15" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="F15"/>
+      <c r="G15" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="H15"/>
+      <c r="K15" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="N15" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16"/>
+      <c r="C16" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="D16"/>
+      <c r="E16" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="F16"/>
+      <c r="G16" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="H16"/>
+      <c r="K16" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="N16" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17"/>
+      <c r="C17" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="D17"/>
+      <c r="E17" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="H17"/>
+      <c r="K17" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18"/>
+      <c r="C18" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D18"/>
+      <c r="E18" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H18"/>
+      <c r="K18" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19"/>
+      <c r="C19" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="F19"/>
+      <c r="G19" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="H19"/>
+      <c r="K19" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20"/>
+      <c r="D20"/>
+      <c r="E20" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="H20"/>
+      <c r="K20" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21"/>
+      <c r="D21"/>
+      <c r="E21" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="F21"/>
+      <c r="H21"/>
+      <c r="M21" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22"/>
+      <c r="D22"/>
+      <c r="E22" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="F22"/>
+      <c r="H22"/>
+      <c r="M22" s="7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23"/>
+      <c r="D23"/>
+      <c r="E23" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="F23"/>
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24"/>
+      <c r="D24"/>
+      <c r="E24" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="F24"/>
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25"/>
+      <c r="D25"/>
+      <c r="E25" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="F25"/>
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26"/>
+      <c r="D26"/>
+      <c r="E26" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="F26"/>
+      <c r="G26" s="7"/>
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27"/>
+      <c r="D27"/>
+      <c r="E27" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="F27"/>
+      <c r="G27" s="7"/>
+      <c r="H27"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28"/>
+      <c r="D28"/>
+      <c r="E28" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="F28"/>
+      <c r="G28" s="7"/>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29"/>
+      <c r="D29"/>
+      <c r="E29" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="F29"/>
+      <c r="G29" s="7"/>
+      <c r="H29"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30"/>
+      <c r="D30"/>
+      <c r="E30" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="F30"/>
+      <c r="G30" s="7"/>
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31"/>
+      <c r="D31"/>
+      <c r="E31" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="F31"/>
+      <c r="G31" s="7"/>
+      <c r="H31"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32"/>
+      <c r="D32"/>
+      <c r="F32"/>
+      <c r="G32" s="7"/>
+      <c r="H32"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33"/>
+      <c r="D33"/>
+      <c r="F33"/>
+      <c r="G33" s="7"/>
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34"/>
+      <c r="D34"/>
+      <c r="F34"/>
+      <c r="G34" s="7"/>
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35"/>
+      <c r="D35"/>
+      <c r="F35"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36"/>
+      <c r="D36"/>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37"/>
+      <c r="D37"/>
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38"/>
+      <c r="D38"/>
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39"/>
+      <c r="D39"/>
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40"/>
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41"/>
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B48"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B50"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E52" s="7"/>
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C53" s="7"/>
+      <c r="D53"/>
+      <c r="E53" s="7"/>
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C54" s="7"/>
+      <c r="D54"/>
+      <c r="E54" s="7"/>
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C55" s="7"/>
+      <c r="D55"/>
+      <c r="E55" s="7"/>
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C56" s="7"/>
+      <c r="D56"/>
+      <c r="E56" s="7"/>
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C57" s="7"/>
+      <c r="D57"/>
+      <c r="E57" s="7"/>
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C58" s="7"/>
+      <c r="D58"/>
+      <c r="E58" s="7"/>
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C59" s="7"/>
+      <c r="D59"/>
+      <c r="E59" s="7"/>
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60"/>
+      <c r="E60" s="7"/>
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61"/>
+      <c r="E61" s="7"/>
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62"/>
+      <c r="E62" s="7"/>
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63"/>
+      <c r="E63" s="7"/>
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64"/>
+      <c r="E64" s="7"/>
+      <c r="F64"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65"/>
+      <c r="E65" s="7"/>
+      <c r="F65"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66"/>
+      <c r="E66" s="7"/>
+      <c r="F66"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67"/>
+      <c r="E67" s="7"/>
+      <c r="F67"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68"/>
+      <c r="E68" s="7"/>
+      <c r="F68"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69"/>
+      <c r="E69" s="7"/>
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70"/>
+      <c r="E70" s="7"/>
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E71" s="7"/>
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F72"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F73"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F74"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C75" s="7"/>
+      <c r="F75"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F76"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F77"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F78"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F79"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F80"/>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F81"/>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F82"/>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F83"/>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F85"/>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F86"/>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F87"/>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F88"/>
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F89"/>
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F90"/>
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F91"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDD6BF5-C159-4766-92DA-0E15E04E773E}">
   <dimension ref="A1:E34"/>
   <sheetViews>
@@ -3088,8 +4130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A702005-EDFB-45BE-A884-6A9A5FF3F0F1}">
   <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3301,6 +4343,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DB6969-FCD4-4AC0-8731-C3FC2B56364B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD53744-91AA-45F2-BD5B-D22DA6D78137}">
   <dimension ref="A1:E34"/>
   <sheetViews>
@@ -3582,7 +4647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59C213A-05F4-4841-BAEC-85842C4D1CD7}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -3644,7 +4709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3BCABF-0B84-4F1D-A86D-03D73AE2839E}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -3886,7 +4951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FB94A1-E8D6-4BE6-B882-526070DB15E4}">
   <dimension ref="A1:C51"/>
   <sheetViews>
@@ -4389,7 +5454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182267D9-48FB-4237-A38C-E4622CDC8171}">
   <dimension ref="A1:D127"/>
   <sheetViews>
@@ -5579,7 +6644,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFF5CF3-7111-4487-862F-A50707F309E6}">
   <dimension ref="A1:C132"/>
   <sheetViews>
@@ -6045,1042 +7110,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6B3CDC-0AFC-4B53-A9D5-8ABE836A7404}">
-  <dimension ref="A1:N91"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.7109375" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="D2" t="s">
-        <v>341</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="F2" t="s">
-        <v>341</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="H2" t="s">
-        <v>341</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="J2" t="s">
-        <v>341</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="L2" t="s">
-        <v>341</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="N2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3"/>
-      <c r="C3" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="D3" t="s">
-        <v>341</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="F3" t="s">
-        <v>341</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="H3" t="s">
-        <v>341</v>
-      </c>
-      <c r="I3" s="7"/>
-      <c r="J3" t="s">
-        <v>341</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="L3" t="s">
-        <v>341</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>420</v>
-      </c>
-      <c r="N3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4"/>
-      <c r="C4" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="D4" t="s">
-        <v>341</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="F4" t="s">
-        <v>341</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="H4" t="s">
-        <v>341</v>
-      </c>
-      <c r="I4" s="7"/>
-      <c r="J4" t="s">
-        <v>341</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="L4" t="s">
-        <v>341</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="N4" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5"/>
-      <c r="C5" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="D5" t="s">
-        <v>341</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="F5" t="s">
-        <v>341</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="H5" t="s">
-        <v>341</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="J5"/>
-      <c r="K5" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="L5" t="s">
-        <v>341</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="N5" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6"/>
-      <c r="C6" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="D6" t="s">
-        <v>341</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="F6"/>
-      <c r="G6" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="H6" t="s">
-        <v>341</v>
-      </c>
-      <c r="I6" s="7"/>
-      <c r="J6"/>
-      <c r="K6" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="L6" t="s">
-        <v>341</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>423</v>
-      </c>
-      <c r="N6" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7"/>
-      <c r="C7" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="D7" t="s">
-        <v>341</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="F7"/>
-      <c r="G7" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="H7" t="s">
-        <v>341</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="J7"/>
-      <c r="K7" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="L7" t="s">
-        <v>341</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>424</v>
-      </c>
-      <c r="N7" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8"/>
-      <c r="C8" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="D8" t="s">
-        <v>341</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="F8"/>
-      <c r="G8" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="H8" t="s">
-        <v>341</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8"/>
-      <c r="K8" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="L8" t="s">
-        <v>341</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>425</v>
-      </c>
-      <c r="N8" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9"/>
-      <c r="C9" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="D9" t="s">
-        <v>341</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="F9"/>
-      <c r="G9" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="H9"/>
-      <c r="I9" s="7"/>
-      <c r="K9" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="L9" t="s">
-        <v>341</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="N9" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10"/>
-      <c r="C10" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="D10" t="s">
-        <v>341</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>393</v>
-      </c>
-      <c r="F10"/>
-      <c r="G10" s="7" t="s">
-        <v>402</v>
-      </c>
-      <c r="H10"/>
-      <c r="I10" s="7"/>
-      <c r="K10" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="L10" t="s">
-        <v>341</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>427</v>
-      </c>
-      <c r="N10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11"/>
-      <c r="C11" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="D11" t="s">
-        <v>341</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="F11"/>
-      <c r="G11" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="H11"/>
-      <c r="K11" s="10" t="s">
-        <v>331</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="N11" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12"/>
-      <c r="C12" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="D12" t="s">
-        <v>341</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>391</v>
-      </c>
-      <c r="F12"/>
-      <c r="G12" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="H12"/>
-      <c r="K12" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="N12" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13"/>
-      <c r="C13" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="D13"/>
-      <c r="E13" s="7" t="s">
-        <v>390</v>
-      </c>
-      <c r="F13"/>
-      <c r="G13" s="7" t="s">
-        <v>410</v>
-      </c>
-      <c r="H13"/>
-      <c r="K13" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>430</v>
-      </c>
-      <c r="N13" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14"/>
-      <c r="C14" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="D14"/>
-      <c r="E14" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="F14"/>
-      <c r="G14" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="H14"/>
-      <c r="K14" s="10" t="s">
-        <v>334</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="N14" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15"/>
-      <c r="C15" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="D15"/>
-      <c r="E15" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="F15"/>
-      <c r="G15" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="H15"/>
-      <c r="K15" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>432</v>
-      </c>
-      <c r="N15" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16"/>
-      <c r="C16" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="D16"/>
-      <c r="E16" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="F16"/>
-      <c r="G16" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="H16"/>
-      <c r="K16" s="10" t="s">
-        <v>336</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>433</v>
-      </c>
-      <c r="N16" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17"/>
-      <c r="C17" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="D17"/>
-      <c r="E17" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="F17"/>
-      <c r="G17" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="H17"/>
-      <c r="K17" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18"/>
-      <c r="C18" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="D18"/>
-      <c r="E18" s="7" t="s">
-        <v>385</v>
-      </c>
-      <c r="F18"/>
-      <c r="G18" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="H18"/>
-      <c r="K18" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="M18" s="7" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19"/>
-      <c r="C19" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="D19"/>
-      <c r="E19" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="F19"/>
-      <c r="G19" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="H19"/>
-      <c r="K19" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20"/>
-      <c r="D20"/>
-      <c r="E20" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="F20"/>
-      <c r="G20" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="H20"/>
-      <c r="K20" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="M20" s="7" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21"/>
-      <c r="D21"/>
-      <c r="E21" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="F21"/>
-      <c r="H21"/>
-      <c r="M21" s="7" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22"/>
-      <c r="D22"/>
-      <c r="E22" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="F22"/>
-      <c r="H22"/>
-      <c r="M22" s="7" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23"/>
-      <c r="D23"/>
-      <c r="E23" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="F23"/>
-      <c r="H23"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24"/>
-      <c r="D24"/>
-      <c r="E24" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="F24"/>
-      <c r="H24"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25"/>
-      <c r="D25"/>
-      <c r="E25" s="7" t="s">
-        <v>378</v>
-      </c>
-      <c r="F25"/>
-      <c r="H25"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26"/>
-      <c r="D26"/>
-      <c r="E26" s="7" t="s">
-        <v>377</v>
-      </c>
-      <c r="F26"/>
-      <c r="G26" s="7"/>
-      <c r="H26"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27"/>
-      <c r="D27"/>
-      <c r="E27" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="F27"/>
-      <c r="G27" s="7"/>
-      <c r="H27"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28"/>
-      <c r="D28"/>
-      <c r="E28" s="7" t="s">
-        <v>375</v>
-      </c>
-      <c r="F28"/>
-      <c r="G28" s="7"/>
-      <c r="H28"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29"/>
-      <c r="D29"/>
-      <c r="E29" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="F29"/>
-      <c r="G29" s="7"/>
-      <c r="H29"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30"/>
-      <c r="D30"/>
-      <c r="E30" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="F30"/>
-      <c r="G30" s="7"/>
-      <c r="H30"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31"/>
-      <c r="D31"/>
-      <c r="E31" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="F31"/>
-      <c r="G31" s="7"/>
-      <c r="H31"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32"/>
-      <c r="D32"/>
-      <c r="F32"/>
-      <c r="G32" s="7"/>
-      <c r="H32"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33"/>
-      <c r="D33"/>
-      <c r="F33"/>
-      <c r="G33" s="7"/>
-      <c r="H33"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34"/>
-      <c r="D34"/>
-      <c r="F34"/>
-      <c r="G34" s="7"/>
-      <c r="H34"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35"/>
-      <c r="D35"/>
-      <c r="F35"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36"/>
-      <c r="D36"/>
-      <c r="F36"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37"/>
-      <c r="D37"/>
-      <c r="F37"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38"/>
-      <c r="D38"/>
-      <c r="F38"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39"/>
-      <c r="D39"/>
-      <c r="F39"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40"/>
-      <c r="D40"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41"/>
-      <c r="D41"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B47"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B48"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B49"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B50"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E52" s="7"/>
-      <c r="F52"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="7"/>
-      <c r="D53"/>
-      <c r="E53" s="7"/>
-      <c r="F53"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C54" s="7"/>
-      <c r="D54"/>
-      <c r="E54" s="7"/>
-      <c r="F54"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C55" s="7"/>
-      <c r="D55"/>
-      <c r="E55" s="7"/>
-      <c r="F55"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="7"/>
-      <c r="D56"/>
-      <c r="E56" s="7"/>
-      <c r="F56"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="7"/>
-      <c r="D57"/>
-      <c r="E57" s="7"/>
-      <c r="F57"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C58" s="7"/>
-      <c r="D58"/>
-      <c r="E58" s="7"/>
-      <c r="F58"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C59" s="7"/>
-      <c r="D59"/>
-      <c r="E59" s="7"/>
-      <c r="F59"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60"/>
-      <c r="E60" s="7"/>
-      <c r="F60"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61"/>
-      <c r="E61" s="7"/>
-      <c r="F61"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62"/>
-      <c r="E62" s="7"/>
-      <c r="F62"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63"/>
-      <c r="E63" s="7"/>
-      <c r="F63"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64"/>
-      <c r="E64" s="7"/>
-      <c r="F64"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65"/>
-      <c r="E65" s="7"/>
-      <c r="F65"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66"/>
-      <c r="E66" s="7"/>
-      <c r="F66"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67"/>
-      <c r="E67" s="7"/>
-      <c r="F67"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68"/>
-      <c r="E68" s="7"/>
-      <c r="F68"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
-      <c r="C69" s="7"/>
-      <c r="D69"/>
-      <c r="E69" s="7"/>
-      <c r="F69"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70"/>
-      <c r="E70" s="7"/>
-      <c r="F70"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E71" s="7"/>
-      <c r="F71"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F72"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F73"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F74"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C75" s="7"/>
-      <c r="F75"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F76"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F77"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F78"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F79"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F80"/>
-    </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F81"/>
-    </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F82"/>
-    </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F83"/>
-    </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F84"/>
-    </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F85"/>
-    </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F86"/>
-    </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F87"/>
-    </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F88"/>
-    </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F89"/>
-    </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F90"/>
-    </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F91"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Code changes done in NAC data flow
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/qa7/testData.xlsx
+++ b/src/test/resources/test-data/qa7/testData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vigneshwaran.sesurag\Gradle\CPP_Automation-Chatr\src\test\resources\test-data\qa7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vigneshwaran.sesurag\Gradle\CPP_Automation-Chatr(Clone)\src\test\resources\test-data\qa7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000A5E55-DD4F-4251-A043-D568C0F4CBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBBE881-78C6-447C-93CA-6AF8B75A42DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="578">
   <si>
     <t>Voucher25</t>
   </si>
@@ -1770,6 +1770,18 @@
   </si>
   <si>
     <t>Chatr@123</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>72</t>
   </si>
 </sst>
 </file>
@@ -5529,10 +5541,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9A6D5F-4ADD-40C7-BC29-FB462C3271E9}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5676,15 +5688,117 @@
       </c>
     </row>
     <row r="4" spans="1:14">
+      <c r="A4" s="12" t="s">
+        <v>567</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>574</v>
+      </c>
       <c r="C4" s="5" t="s">
-        <v>572</v>
+        <v>545</v>
+      </c>
+      <c r="D4" t="s">
+        <v>552</v>
+      </c>
+      <c r="E4" t="s">
+        <v>575</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="G4" t="s">
+        <v>557</v>
+      </c>
+      <c r="H4" t="s">
+        <v>562</v>
+      </c>
+      <c r="I4" t="s">
+        <v>563</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="K4" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="12" t="s">
+        <v>567</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="D5" t="s">
+        <v>552</v>
+      </c>
+      <c r="E5" t="s">
+        <v>575</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="G5" t="s">
+        <v>557</v>
+      </c>
+      <c r="H5" t="s">
+        <v>562</v>
+      </c>
+      <c r="I5" t="s">
+        <v>563</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="K5" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="12" t="s">
+        <v>567</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="D6" t="s">
+        <v>552</v>
+      </c>
+      <c r="E6" t="s">
+        <v>575</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="G6" t="s">
+        <v>557</v>
+      </c>
+      <c r="H6" t="s">
+        <v>562</v>
+      </c>
+      <c r="I6" t="s">
+        <v>563</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="K6" t="s">
+        <v>565</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{3C80A37F-1BB2-4ED7-9BFE-1B1BF601C38C}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{F1D2BB13-1C81-4D90-8542-1476FF315AA6}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{379E461C-6E89-4160-A918-B8DAD61334CD}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{90B198B2-6FF2-4768-865C-4AE2F22D091E}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{78C3D959-BCE9-44C1-A054-62DE769C62A4}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{088FD480-FD89-44BB-B837-33D1A6A2BE5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5697,7 +5811,16 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="5" t="s">
+        <v>572</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{379E461C-6E89-4160-A918-B8DAD61334CD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>